<commit_message>
HEEDLS-565 Update the formatting on the date, number and bool columns
</commit_message>
<xml_diff>
--- a/DigitalLearningSolutions.Data.Tests/TestData/CourseDelegateExportCurrentDataDownloadTest.xlsx
+++ b/DigitalLearningSolutions.Data.Tests/TestData/CourseDelegateExportCurrentDataDownloadTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alejac\Git\DLSV2\DigitalLearningSolutions.Data.Tests\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80448C6F-DB24-49A9-95A2-A732500A4433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853EA64F-D1DA-4242-829C-14C8AB00EE4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23136" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Last name</t>
   </si>
@@ -106,21 +106,6 @@
     <t>TM68</t>
   </si>
   <si>
-    <t>24/05/2012 00:00:00</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
     <t>Bennett</t>
   </si>
   <si>
@@ -139,18 +124,6 @@
     <t>ES1</t>
   </si>
   <si>
-    <t>22/09/2010 00:00:00</t>
-  </si>
-  <si>
-    <t>08/03/2018 00:00:00</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
     <t>Griffin</t>
   </si>
   <si>
@@ -164,15 +137,15 @@
   </si>
   <si>
     <t>NB8</t>
-  </si>
-  <si>
-    <t>22/03/2011 00:00:00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,10 +182,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -549,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,132 +641,136 @@
       <c r="I2" t="s">
         <v>27</v>
       </c>
-      <c r="J2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K2" t="s">
-        <v>40</v>
-      </c>
-      <c r="N2" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" t="s">
-        <v>31</v>
-      </c>
-      <c r="U2" t="s">
-        <v>32</v>
+      <c r="J2" s="5">
+        <v>41053</v>
+      </c>
+      <c r="K2" s="4">
+        <v>43167</v>
+      </c>
+      <c r="L2" s="5"/>
+      <c r="M2" s="4"/>
+      <c r="N2">
+        <v>2</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P3" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>41</v>
-      </c>
-      <c r="R3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" t="s">
-        <v>32</v>
+      <c r="J3" s="5">
+        <v>40443</v>
+      </c>
+      <c r="K3" s="5">
+        <v>43167</v>
+      </c>
+      <c r="L3" s="5"/>
+      <c r="M3" s="4">
+        <v>43167</v>
+      </c>
+      <c r="N3">
+        <v>2</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>100</v>
+      </c>
+      <c r="S3" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U3" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
         <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" t="s">
-        <v>40</v>
-      </c>
-      <c r="N4" t="s">
-        <v>41</v>
-      </c>
-      <c r="O4" t="s">
-        <v>41</v>
-      </c>
-      <c r="P4" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>41</v>
-      </c>
-      <c r="R4" t="s">
-        <v>42</v>
-      </c>
-      <c r="S4" t="s">
-        <v>31</v>
-      </c>
-      <c r="U4" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="J4" s="5">
+        <v>40624</v>
+      </c>
+      <c r="K4" s="5">
+        <v>43167</v>
+      </c>
+      <c r="L4" s="5"/>
+      <c r="M4" s="4">
+        <v>43167</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>1</v>
+      </c>
+      <c r="R4">
+        <v>100</v>
+      </c>
+      <c r="S4" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="U4" s="3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>